<commit_message>
atualiza script e documentação
</commit_message>
<xml_diff>
--- a/planilhas_tratadas.xlsx
+++ b/planilhas_tratadas.xlsx
@@ -348,7 +348,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="A1:J12"/>
@@ -821,22 +821,29 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PORCENT_COMPLETA (%)</t>
-        </is>
-      </c>
-      <c r="B13" s="4">
-        <f>COUNT(B4:J11) / COUNTA(B4:J11)</f>
-        <v/>
+          <t>-------------</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>PORCENT_COMPLETA (%)</t>
+        </is>
+      </c>
+      <c r="B14" s="4">
+        <f>COUNT(B4:J11) / COUNTA(B4:J11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>PORCENT_AUSENTE (%)</t>
         </is>
       </c>
-      <c r="B14" s="4">
-        <f>1-B13</f>
+      <c r="B15" s="4">
+        <f>1-B14</f>
         <v/>
       </c>
     </row>
@@ -851,7 +858,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -1115,22 +1122,29 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PORCENT_COMPLETA (%)</t>
-        </is>
-      </c>
-      <c r="B10" s="4">
-        <f>COUNT(B4:G8) / COUNTA(B4:G8)</f>
-        <v/>
+          <t>-------------</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>PORCENT_COMPLETA (%)</t>
+        </is>
+      </c>
+      <c r="B11" s="4">
+        <f>COUNT(B4:G8) / COUNTA(B4:G8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>PORCENT_AUSENTE (%)</t>
         </is>
       </c>
-      <c r="B11" s="4">
-        <f>1-B10</f>
+      <c r="B12" s="4">
+        <f>1-B11</f>
         <v/>
       </c>
     </row>
@@ -1145,7 +1159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
@@ -1311,22 +1325,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PORCENT_COMPLETA (%)</t>
-        </is>
-      </c>
-      <c r="B9" s="4">
-        <f>COUNT(B4:D7) / COUNTA(B4:D7)</f>
-        <v/>
+          <t>-------------</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>PORCENT_COMPLETA (%)</t>
+        </is>
+      </c>
+      <c r="B10" s="4">
+        <f>COUNT(B4:D7) / COUNTA(B4:D7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>PORCENT_AUSENTE (%)</t>
         </is>
       </c>
-      <c r="B10" s="4">
-        <f>1-B9</f>
+      <c r="B11" s="4">
+        <f>1-B10</f>
         <v/>
       </c>
     </row>
@@ -1341,7 +1362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -1820,22 +1841,29 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PORCENT_COMPLETA (%)</t>
-        </is>
-      </c>
-      <c r="B14" s="4">
-        <f>COUNT(B5:J12) / COUNTA(B5:J12)</f>
-        <v/>
+          <t>-------------</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>PORCENT_COMPLETA (%)</t>
+        </is>
+      </c>
+      <c r="B15" s="4">
+        <f>COUNT(B5:J12) / COUNTA(B5:J12)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>PORCENT_AUSENTE (%)</t>
         </is>
       </c>
-      <c r="B15" s="4">
-        <f>1-B14</f>
+      <c r="B16" s="4">
+        <f>1-B15</f>
         <v/>
       </c>
     </row>

</xml_diff>